<commit_message>
changed N/a to no sector
</commit_message>
<xml_diff>
--- a/data/sector_correlations/2010_intra.xlsx
+++ b/data/sector_correlations/2010_intra.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,461 +458,461 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Multiline Retail(8)</t>
+          <t>Multiline Retail(7)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6150161039582829</v>
+        <v>0.637158856603528</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Multi-Utilities(19)</t>
+          <t>Multi-Utilities(18)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5695496049093012</v>
+        <v>0.5909373411224138</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Auto Components(21)</t>
+          <t>Containers &amp; Packaging(12)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5537157241117897</v>
+        <v>0.5820552138888447</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Road &amp; Rail(23)</t>
+          <t>Machinery(85)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5221321907756564</v>
+        <v>0.5773156141689123</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Machinery(93)</t>
+          <t>Road &amp; Rail(22)</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5008207950999281</v>
+        <v>0.5710044321418385</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Energy Equipment &amp; Services(34)</t>
+          <t>Auto Components(21)</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4924166702414297</v>
+        <v>0.5537157241117897</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gas Utilities(13)</t>
+          <t>Air Freight &amp; Logistics(11)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.4875253763803912</v>
+        <v>0.5118791143994464</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hotels, Restaurants &amp; Leisure(54)</t>
+          <t>Energy Equipment &amp; Services(32)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4837938333975689</v>
+        <v>0.5006236236380753</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Air Freight &amp; Logistics(12)</t>
+          <t>Electric Utilities(28)</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.4811146901603654</v>
+        <v>0.5001381885300904</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Airlines(15)</t>
+          <t>Airlines(14)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.4779684341012124</v>
+        <v>0.4917499218936111</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Wireless Telecommunication Services(14)</t>
+          <t>Specialty Retail(58)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4702411239861925</v>
+        <v>0.4879427848495779</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Electric Utilities(29)</t>
+          <t>Trading Companies &amp; Distributors(25)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4401267292830536</v>
+        <v>0.4854130637614995</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chemicals(55)</t>
+          <t>Gas Utilities(12)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.4356510290946238</v>
+        <v>0.4786730779818642</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Specialty Retail(63)</t>
+          <t>Wireless Telecommunication Services(14)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.4325546482786442</v>
+        <v>0.4702411239861925</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Trading Companies &amp; Distributors(28)</t>
+          <t>Hotels, Restaurants &amp; Leisure(50)</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.4321899605282879</v>
+        <v>0.4685900344946026</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Containers &amp; Packaging(14)</t>
+          <t>Chemicals(51)</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.4182623626803931</v>
+        <v>0.4634824288800502</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Leisure Products(12)</t>
+          <t>Media(42)</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.4084067807890574</v>
+        <v>0.4632595642572921</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Household Products(10)</t>
+          <t>Construction &amp; Engineering(20)</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.4064015974987705</v>
+        <v>0.4551704769440679</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Interactive Media &amp; Services(11)</t>
+          <t>Semiconductors &amp; Semiconductor Equipment(68)</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.3800458486065889</v>
+        <v>0.4341880161375474</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Household Durables(43)</t>
+          <t>Leisure Products(11)</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.3788740673641546</v>
+        <v>0.4273113347199632</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Aerospace &amp; Defense(43)</t>
+          <t>Building Products(23)</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.3702874806657651</v>
+        <v>0.4193499308950515</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Insurance(80)</t>
+          <t>Household Durables(39)</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.3662579085491515</v>
+        <v>0.4173637377507899</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Marine(16)</t>
+          <t>Capital Markets(75)</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.3646892218307625</v>
+        <v>0.4068347560461073</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Oil, Gas &amp; Consumable Fuels(128)</t>
+          <t>Household Products(10)</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.3643032934481281</v>
+        <v>0.4064015974987705</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Water Utilities(13)</t>
+          <t>Marine(15)</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.3587291924488062</v>
+        <v>0.4033073324332358</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Diversified Consumer Services(18)</t>
+          <t>Aerospace &amp; Defense(37)</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.3543355357849205</v>
+        <v>0.3975633353773633</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Media(47)</t>
+          <t>Communications Equipment(45)</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.3519937362825795</v>
+        <v>0.3803307251461573</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Capital Markets(87)</t>
+          <t>Oil, Gas &amp; Consumable Fuels(122)</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.3425595084734919</v>
+        <v>0.3755636762179344</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Commercial Services &amp; Supplies(57)</t>
+          <t>Insurance(75)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3409304223354978</v>
+        <v>0.3678833024531595</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Semiconductors &amp; Semiconductor Equipment(75)</t>
+          <t>Commercial Services &amp; Supplies(52)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.3408765740580432</v>
+        <v>0.3607899127967236</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Diversified Telecommunication Services(21)</t>
+          <t>Consumer Finance(15)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.3407785325465063</v>
+        <v>0.3521445803575914</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Communications Equipment(50)</t>
+          <t>Textiles, Apparel &amp; Luxury Goods(29)</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.3204888748182637</v>
+        <v>0.3515114243143465</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Textiles, Apparel &amp; Luxury Goods(30)</t>
+          <t>Diversified Consumer Services(17)</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.31917389331533</v>
+        <v>0.3499089347939527</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Electrical Equipment(31)</t>
+          <t>Metals &amp; Mining(89)</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.3190851922723622</v>
+        <v>0.3388671756232035</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Construction &amp; Engineering(23)</t>
+          <t>Water Utilities(12)</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.3187887796852782</v>
+        <v>0.3368986889980476</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Blank Check / SPAC(32)</t>
+          <t>Diversified Telecommunication Services(20)</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.3127988268276335</v>
+        <v>0.3291281176173813</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Metals &amp; Mining(95)</t>
+          <t>Professional Services(35)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.3065005256736139</v>
+        <v>0.3241847688660761</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Internet &amp; Direct Marketing Retail(19)</t>
+          <t>Electrical Equipment(28)</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.3039055664368063</v>
+        <v>0.3177397643706062</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Food &amp; Staples Retailing(15)</t>
+          <t>Life Sciences Tools &amp; Services(19)</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.3026795069584989</v>
+        <v>0.3115688160483179</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Building Products(27)</t>
+          <t>Banks(246)</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.302478630459339</v>
+        <v>0.3029498278140831</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Life Sciences Tools &amp; Services(20)</t>
+          <t>Food &amp; Staples Retailing(15)</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.3015216866281789</v>
+        <v>0.3026795069584989</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Professional Services(38)</t>
+          <t>Software(66)</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.2953660850180291</v>
+        <v>0.2980981953635595</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Shell Companies(18)</t>
+          <t>Internet &amp; Direct Marketing Retail(15)</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.2945975286587432</v>
+        <v>0.2952069581098644</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Software(70)</t>
+          <t>Health Care Providers &amp; Services(46)</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.2820893074913978</v>
+        <v>0.2907406161623396</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Health Care Providers &amp; Services(48)</t>
+          <t>IT Services(52)</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.2813180400864438</v>
+        <v>0.2895560816946511</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Beverages(22)</t>
+          <t>Beverages(21)</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.2707693607078286</v>
+        <v>0.270311358287111</v>
       </c>
     </row>
     <row r="49">
@@ -928,101 +928,61 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Banks(271)</t>
+          <t>Health Care Equipment &amp; Supplies(83)</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.2581496642577882</v>
+        <v>0.2530052926919384</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>IT Services(58)</t>
+          <t>Thrifts &amp; Mortgage Finance(47)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.256885814821021</v>
+        <v>0.2454875116583609</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Entertainment(26)</t>
+          <t>Entertainment(22)</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.2514116667082163</v>
+        <v>0.2426693261706819</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Health Care Equipment &amp; Supplies(87)</t>
+          <t>Food Products(44)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.2445660720724388</v>
+        <v>0.1977162084373913</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Consumer Finance(23)</t>
+          <t>Pharmaceuticals(48)</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.2410224384792897</v>
+        <v>0.1616154705497828</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Thrifts &amp; Mortgage Finance(52)</t>
+          <t>Biotechnology(126)</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.1819448699576301</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Pharmaceuticals(56)</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>0.1748667326312322</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Real Estate Management &amp; Development(28)</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>0.1731128703745456</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Food Products(47)</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>0.1600494406099215</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Biotechnology(163)</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>0.1396019068816015</v>
+        <v>0.1573268451086477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New changes in main
</commit_message>
<xml_diff>
--- a/data/sector_correlations/2010_intra.xlsx
+++ b/data/sector_correlations/2010_intra.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,461 +458,461 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Multiline Retail(8)</t>
+          <t>Multiline Retail(7)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6150161039582829</v>
+        <v>0.637158856603528</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Multi-Utilities(19)</t>
+          <t>Multi-Utilities(18)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5695496049093012</v>
+        <v>0.5909373411224138</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Auto Components(21)</t>
+          <t>Containers &amp; Packaging(12)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5537157241117897</v>
+        <v>0.5820552138888447</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Road &amp; Rail(23)</t>
+          <t>Machinery(85)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5221321907756564</v>
+        <v>0.5773156141689123</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Machinery(93)</t>
+          <t>Road &amp; Rail(22)</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5008207950999281</v>
+        <v>0.5710044321418385</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Energy Equipment &amp; Services(34)</t>
+          <t>Auto Components(21)</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4924166702414297</v>
+        <v>0.5537157241117897</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gas Utilities(13)</t>
+          <t>Air Freight &amp; Logistics(11)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.4875253763803912</v>
+        <v>0.5118791143994464</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hotels, Restaurants &amp; Leisure(54)</t>
+          <t>Energy Equipment &amp; Services(32)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4837938333975689</v>
+        <v>0.5006236236380753</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Air Freight &amp; Logistics(12)</t>
+          <t>Electric Utilities(28)</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.4811146901603654</v>
+        <v>0.5001381885300904</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Airlines(15)</t>
+          <t>Airlines(14)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.4779684341012124</v>
+        <v>0.4917499218936111</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Wireless Telecommunication Services(14)</t>
+          <t>Specialty Retail(58)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4702411239861925</v>
+        <v>0.4879427848495779</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Electric Utilities(29)</t>
+          <t>Trading Companies &amp; Distributors(25)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4401267292830536</v>
+        <v>0.4854130637614995</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chemicals(55)</t>
+          <t>Gas Utilities(12)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.4356510290946238</v>
+        <v>0.4786730779818642</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Specialty Retail(63)</t>
+          <t>Wireless Telecommunication Services(14)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.4325546482786442</v>
+        <v>0.4702411239861925</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Trading Companies &amp; Distributors(28)</t>
+          <t>Hotels, Restaurants &amp; Leisure(50)</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.4321899605282879</v>
+        <v>0.4685900344946026</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Containers &amp; Packaging(14)</t>
+          <t>Chemicals(51)</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.4182623626803931</v>
+        <v>0.4634824288800502</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Leisure Products(12)</t>
+          <t>Media(42)</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.4084067807890574</v>
+        <v>0.4632595642572921</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Household Products(10)</t>
+          <t>Construction &amp; Engineering(20)</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.4064015974987705</v>
+        <v>0.4551704769440679</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Interactive Media &amp; Services(11)</t>
+          <t>Semiconductors &amp; Semiconductor Equipment(68)</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.3800458486065889</v>
+        <v>0.4341880161375474</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Household Durables(43)</t>
+          <t>Leisure Products(11)</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.3788740673641546</v>
+        <v>0.4273113347199632</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Aerospace &amp; Defense(43)</t>
+          <t>Building Products(23)</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.3702874806657651</v>
+        <v>0.4193499308950515</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Insurance(80)</t>
+          <t>Household Durables(39)</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.3662579085491515</v>
+        <v>0.4173637377507899</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Marine(16)</t>
+          <t>Capital Markets(75)</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.3646892218307625</v>
+        <v>0.4068347560461073</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Oil, Gas &amp; Consumable Fuels(128)</t>
+          <t>Household Products(10)</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.3643032934481281</v>
+        <v>0.4064015974987705</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Water Utilities(13)</t>
+          <t>Marine(15)</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.3587291924488062</v>
+        <v>0.4033073324332358</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Diversified Consumer Services(18)</t>
+          <t>Aerospace &amp; Defense(37)</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.3543355357849205</v>
+        <v>0.3975633353773633</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Media(47)</t>
+          <t>Communications Equipment(45)</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.3519937362825795</v>
+        <v>0.3803307251461573</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Capital Markets(87)</t>
+          <t>Oil, Gas &amp; Consumable Fuels(122)</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.3425595084734919</v>
+        <v>0.3755636762179344</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Commercial Services &amp; Supplies(57)</t>
+          <t>Insurance(75)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3409304223354978</v>
+        <v>0.3678833024531595</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Semiconductors &amp; Semiconductor Equipment(75)</t>
+          <t>Commercial Services &amp; Supplies(52)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.3408765740580432</v>
+        <v>0.3607899127967236</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Diversified Telecommunication Services(21)</t>
+          <t>Consumer Finance(15)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.3407785325465063</v>
+        <v>0.3521445803575914</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Communications Equipment(50)</t>
+          <t>Textiles, Apparel &amp; Luxury Goods(29)</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.3204888748182637</v>
+        <v>0.3515114243143465</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Textiles, Apparel &amp; Luxury Goods(30)</t>
+          <t>Diversified Consumer Services(17)</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.31917389331533</v>
+        <v>0.3499089347939527</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Electrical Equipment(31)</t>
+          <t>Metals &amp; Mining(89)</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.3190851922723622</v>
+        <v>0.3388671756232035</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Construction &amp; Engineering(23)</t>
+          <t>Water Utilities(12)</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.3187887796852782</v>
+        <v>0.3368986889980476</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Blank Check / SPAC(32)</t>
+          <t>Diversified Telecommunication Services(20)</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.3127988268276335</v>
+        <v>0.3291281176173813</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Metals &amp; Mining(95)</t>
+          <t>Professional Services(35)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.3065005256736139</v>
+        <v>0.3241847688660761</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Internet &amp; Direct Marketing Retail(19)</t>
+          <t>Electrical Equipment(28)</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.3039055664368063</v>
+        <v>0.3177397643706062</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Food &amp; Staples Retailing(15)</t>
+          <t>Life Sciences Tools &amp; Services(19)</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.3026795069584989</v>
+        <v>0.3115688160483179</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Building Products(27)</t>
+          <t>Banks(246)</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.302478630459339</v>
+        <v>0.3029498278140831</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Life Sciences Tools &amp; Services(20)</t>
+          <t>Food &amp; Staples Retailing(15)</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.3015216866281789</v>
+        <v>0.3026795069584989</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Professional Services(38)</t>
+          <t>Software(66)</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.2953660850180291</v>
+        <v>0.2980981953635595</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Shell Companies(18)</t>
+          <t>Internet &amp; Direct Marketing Retail(15)</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.2945975286587432</v>
+        <v>0.2952069581098644</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Software(70)</t>
+          <t>Health Care Providers &amp; Services(46)</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.2820893074913978</v>
+        <v>0.2907406161623396</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Health Care Providers &amp; Services(48)</t>
+          <t>IT Services(52)</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.2813180400864438</v>
+        <v>0.2895560816946511</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Beverages(22)</t>
+          <t>Beverages(21)</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.2707693607078286</v>
+        <v>0.270311358287111</v>
       </c>
     </row>
     <row r="49">
@@ -928,101 +928,61 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Banks(271)</t>
+          <t>Health Care Equipment &amp; Supplies(83)</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.2581496642577882</v>
+        <v>0.2530052926919384</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>IT Services(58)</t>
+          <t>Thrifts &amp; Mortgage Finance(47)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.256885814821021</v>
+        <v>0.2454875116583609</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Entertainment(26)</t>
+          <t>Entertainment(22)</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.2514116667082163</v>
+        <v>0.2426693261706819</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Health Care Equipment &amp; Supplies(87)</t>
+          <t>Food Products(44)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.2445660720724388</v>
+        <v>0.1977162084373913</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Consumer Finance(23)</t>
+          <t>Pharmaceuticals(48)</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.2410224384792897</v>
+        <v>0.1616154705497828</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Thrifts &amp; Mortgage Finance(52)</t>
+          <t>Biotechnology(126)</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.1819448699576301</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Pharmaceuticals(56)</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>0.1748667326312322</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Real Estate Management &amp; Development(28)</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>0.1731128703745456</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Food Products(47)</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>0.1600494406099215</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Biotechnology(163)</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>0.1396019068816015</v>
+        <v>0.1573268451086477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recalculate all sector comparisons done
</commit_message>
<xml_diff>
--- a/data/sector_correlations/2010_intra.xlsx
+++ b/data/sector_correlations/2010_intra.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,11 +488,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Machinery(85)</t>
+          <t>Machinery(86)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5773156141689123</v>
+        <v>0.574297532791705</v>
       </c>
     </row>
     <row r="7">
@@ -528,191 +528,191 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Energy Equipment &amp; Services(32)</t>
+          <t>Electric Utilities(28)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.5006236236380753</v>
+        <v>0.5001381885300904</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Electric Utilities(28)</t>
+          <t>Airlines(14)</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5001381885300904</v>
+        <v>0.4917499218936111</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Airlines(14)</t>
+          <t>Trading Companies &amp; Distributors(25)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.4917499218936111</v>
+        <v>0.4854130637614995</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Specialty Retail(58)</t>
+          <t>Gas Utilities(12)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4879427848495779</v>
+        <v>0.4786730779818642</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Trading Companies &amp; Distributors(25)</t>
+          <t>Equity Real Estate Investment Trusts ...(98)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4854130637614995</v>
+        <v>0.4718664674272164</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Gas Utilities(12)</t>
+          <t>Hotels, Restaurants &amp; Leisure(51)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.4786730779818642</v>
+        <v>0.47141191301275</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Wireless Telecommunication Services(14)</t>
+          <t>Specialty Retail(59)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.4702411239861925</v>
+        <v>0.4711957565821278</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hotels, Restaurants &amp; Leisure(50)</t>
+          <t>Wireless Telecommunication Services(14)</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.4685900344946026</v>
+        <v>0.4702411239861925</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Chemicals(51)</t>
+          <t>Media(42)</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.4634824288800502</v>
+        <v>0.4632595642572921</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Media(42)</t>
+          <t>Chemicals(52)</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.4632595642572921</v>
+        <v>0.4613830175459043</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Construction &amp; Engineering(20)</t>
+          <t>Construction &amp; Engineering(21)</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.4551704769440679</v>
+        <v>0.45996107255264</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Semiconductors &amp; Semiconductor Equipment(68)</t>
+          <t>Leisure Products(11)</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.4341880161375474</v>
+        <v>0.4273113347199632</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Leisure Products(11)</t>
+          <t>Semiconductors &amp; Semiconductor Equipment(70)</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.4273113347199632</v>
+        <v>0.418425023374555</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Building Products(23)</t>
+          <t>Household Durables(39)</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.4193499308950515</v>
+        <v>0.4173637377507899</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Household Durables(39)</t>
+          <t>Household Products(10)</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.4173637377507899</v>
+        <v>0.4064015974987705</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Capital Markets(75)</t>
+          <t>Marine(15)</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.4068347560461073</v>
+        <v>0.4033073324332358</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Household Products(10)</t>
+          <t>Aerospace &amp; Defense(37)</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.4064015974987705</v>
+        <v>0.3975633353773633</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Marine(15)</t>
+          <t>Building Products(24)</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.4033073324332358</v>
+        <v>0.3962955128265593</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Aerospace &amp; Defense(37)</t>
+          <t>Capital Markets(76)</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.3975633353773633</v>
+        <v>0.3908099843454869</v>
       </c>
     </row>
     <row r="29">
@@ -728,151 +728,151 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Oil, Gas &amp; Consumable Fuels(122)</t>
+          <t>Oil, Gas &amp; Consumable Fuels(125)</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.3755636762179344</v>
+        <v>0.3799339577785524</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Insurance(75)</t>
+          <t>Energy Equipment &amp; Services(38)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3678833024531595</v>
+        <v>0.3737127086805898</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Commercial Services &amp; Supplies(52)</t>
+          <t>Insurance(75)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.3607899127967236</v>
+        <v>0.3678833024531595</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Consumer Finance(15)</t>
+          <t>Technology Hardware, Storage &amp; Periph...(19)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.3521445803575914</v>
+        <v>0.3647382387362086</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Textiles, Apparel &amp; Luxury Goods(29)</t>
+          <t>Commercial Services &amp; Supplies(52)</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.3515114243143465</v>
+        <v>0.3607899127967236</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Diversified Consumer Services(17)</t>
+          <t>Consumer Finance(15)</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.3499089347939527</v>
+        <v>0.3521445803575914</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Metals &amp; Mining(89)</t>
+          <t>Textiles, Apparel &amp; Luxury Goods(29)</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.3388671756232035</v>
+        <v>0.3515114243143465</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Water Utilities(12)</t>
+          <t>Diversified Consumer Services(17)</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.3368986889980476</v>
+        <v>0.3499089347939527</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Diversified Telecommunication Services(20)</t>
+          <t>Water Utilities(13)</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.3291281176173813</v>
+        <v>0.336959255027089</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Professional Services(35)</t>
+          <t>Diversified Telecommunication Services(20)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.3241847688660761</v>
+        <v>0.3291281176173813</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Electrical Equipment(28)</t>
+          <t>ETF(303)</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.3177397643706062</v>
+        <v>0.3252695302660542</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Life Sciences Tools &amp; Services(19)</t>
+          <t>Professional Services(35)</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.3115688160483179</v>
+        <v>0.3241847688660761</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Banks(246)</t>
+          <t>Electrical Equipment(28)</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.3029498278140831</v>
+        <v>0.3177397643706062</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Food &amp; Staples Retailing(15)</t>
+          <t>Life Sciences Tools &amp; Services(19)</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.3026795069584989</v>
+        <v>0.3115688160483179</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Software(66)</t>
+          <t>Electronic Equipment, Instruments &amp; C...(78)</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.2980981953635595</v>
+        <v>0.3103076408935375</v>
       </c>
     </row>
     <row r="45">
@@ -888,11 +888,11 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Health Care Providers &amp; Services(46)</t>
+          <t>Software(70)</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.2907406161623396</v>
+        <v>0.2918107675410762</v>
       </c>
     </row>
     <row r="47">
@@ -908,91 +908,121 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>No Sector(375)</t>
+          <t>Health Care Providers &amp; Services(47)</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.2775156486273571</v>
+        <v>0.2880824409626052</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Beverages(21)</t>
+          <t>Banks(251)</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.270311358287111</v>
+        <v>0.2879755813017612</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Personal Products(19)</t>
+          <t>Food &amp; Staples Retailing(16)</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.2646998600836321</v>
+        <v>0.2841416381203662</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Health Care Equipment &amp; Supplies(83)</t>
+          <t>Beverages(21)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.2530052926919384</v>
+        <v>0.270311358287111</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Thrifts &amp; Mortgage Finance(47)</t>
+          <t>Personal Products(19)</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.2454875116583609</v>
+        <v>0.2646998600836321</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Entertainment(22)</t>
+          <t>Health Care Equipment &amp; Supplies(86)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.2426693261706819</v>
+        <v>0.2526533277781496</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Food Products(44)</t>
+          <t>Metals &amp; Mining(106)</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.1977162084373913</v>
+        <v>0.2491614927465716</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Pharmaceuticals(48)</t>
+          <t>Thrifts &amp; Mortgage Finance(47)</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.1616154705497828</v>
+        <v>0.2454875116583609</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Biotechnology(126)</t>
+          <t>Entertainment(22)</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.1573268451086477</v>
+        <v>0.2426693261706819</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Food Products(46)</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.1892125073366443</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Biotechnology(128)</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.1561710254254096</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Pharmaceuticals(53)</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.154122602581187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>